<commit_message>
630922 Updated for retest of final build at IOC entry
</commit_message>
<xml_diff>
--- a/Test/Build 6/TAS eBill Defect Log IB_2.0_608.xlsx
+++ b/Test/Build 6/TAS eBill Defect Log IB_2.0_608.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaispbalchj\.atlassian-companion\ac29f1f5-0814-40e4-b29f-114adde3bbbf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaispbalchj\Documents\eBilling Docs\Build 5&amp;6\Docs\Defect Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10344" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="176">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -102,21 +102,6 @@
   </si>
   <si>
     <t>US 1909 - Remove Ability to Define Insurance Company as non-EDI</t>
-  </si>
-  <si>
-    <r>
-      <t>Version 1.0</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color indexed="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">               </t>
-    </r>
   </si>
   <si>
     <t>DE487</t>
@@ -589,6 +574,27 @@
   </si>
   <si>
     <t>UAT - CMN Ox question 4  - piece 4 now holds piece 4 and  5</t>
+  </si>
+  <si>
+    <t>October 2018</t>
+  </si>
+  <si>
+    <r>
+      <t>Version 2.0</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">               </t>
+    </r>
+  </si>
+  <si>
+    <t>Updated for Blds 5/6 retesting effort</t>
   </si>
 </sst>
 </file>
@@ -2122,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:H34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2150,7 +2156,7 @@
     </row>
     <row r="7" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
@@ -2204,7 +2210,7 @@
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="46" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="B23" s="46"/>
       <c r="C23" s="46"/>
@@ -2224,7 +2230,7 @@
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="47" t="s">
-        <v>27</v>
+        <v>174</v>
       </c>
       <c r="B26" s="47"/>
       <c r="C26" s="47"/>
@@ -2270,7 +2276,7 @@
   <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2306,7 +2312,7 @@
     </row>
     <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
@@ -2325,10 +2331,18 @@
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="11"/>
+      <c r="A6" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="13">
+        <v>2</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
@@ -2395,7 +2409,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2471,7 +2485,7 @@
         <v>25</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" s="29"/>
     </row>
@@ -2501,19 +2515,19 @@
         <v>25</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>8</v>
@@ -2522,28 +2536,28 @@
         <v>20</v>
       </c>
       <c r="F4" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="28" t="s">
-        <v>31</v>
-      </c>
       <c r="H4" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>8</v>
@@ -2552,58 +2566,58 @@
         <v>20</v>
       </c>
       <c r="F5" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="28" t="s">
         <v>42</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>43</v>
       </c>
       <c r="J5" s="31"/>
     </row>
     <row r="6" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I6" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J6" s="31"/>
     </row>
     <row r="7" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>8</v>
@@ -2612,58 +2626,58 @@
         <v>20</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="28" t="s">
-        <v>39</v>
-      </c>
       <c r="I7" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J7" s="31"/>
     </row>
     <row r="8" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="28" t="s">
         <v>61</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>62</v>
       </c>
       <c r="J8" s="31"/>
     </row>
     <row r="9" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>8</v>
@@ -2672,29 +2686,29 @@
         <v>20</v>
       </c>
       <c r="F9" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="28" t="s">
-        <v>56</v>
-      </c>
       <c r="H9" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I9" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J9" s="40"/>
       <c r="M9" s="42"/>
     </row>
     <row r="10" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>8</v>
@@ -2703,28 +2717,28 @@
         <v>20</v>
       </c>
       <c r="F10" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="28" t="s">
-        <v>56</v>
-      </c>
       <c r="H10" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J10" s="31"/>
     </row>
     <row r="11" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>8</v>
@@ -2733,208 +2747,208 @@
         <v>20</v>
       </c>
       <c r="F11" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="28" t="s">
-        <v>56</v>
-      </c>
       <c r="H11" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J11" s="31"/>
     </row>
     <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J12" s="31"/>
     </row>
     <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I13" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J13" s="31"/>
     </row>
     <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" s="28" t="s">
         <v>96</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>97</v>
       </c>
       <c r="J14" s="31"/>
     </row>
     <row r="15" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" s="36" t="s">
+      <c r="I15" s="28" t="s">
         <v>99</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>100</v>
       </c>
       <c r="J15" s="31"/>
     </row>
     <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="28" t="s">
-        <v>77</v>
-      </c>
       <c r="H16" s="37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I16" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J16" s="31"/>
     </row>
     <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="H17" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="41" t="s">
-        <v>85</v>
-      </c>
       <c r="I17" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>8</v>
@@ -2943,58 +2957,58 @@
         <v>20</v>
       </c>
       <c r="F18" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="H18" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="32" t="s">
-        <v>85</v>
-      </c>
       <c r="I18" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J18" s="31"/>
     </row>
     <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20" s="28" t="s">
         <v>8</v>
@@ -3003,28 +3017,28 @@
         <v>20</v>
       </c>
       <c r="F20" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" s="31" t="s">
         <v>105</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H20" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I20" s="31" t="s">
-        <v>106</v>
       </c>
       <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" s="28" t="s">
         <v>8</v>
@@ -3033,28 +3047,28 @@
         <v>20</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H21" s="37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J21" s="31"/>
     </row>
     <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D22" s="28" t="s">
         <v>8</v>
@@ -3063,28 +3077,28 @@
         <v>20</v>
       </c>
       <c r="F22" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="I22" s="31" t="s">
         <v>113</v>
-      </c>
-      <c r="G22" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="I22" s="31" t="s">
-        <v>114</v>
       </c>
       <c r="J22" s="31"/>
     </row>
     <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D23" s="28" t="s">
         <v>8</v>
@@ -3093,28 +3107,28 @@
         <v>20</v>
       </c>
       <c r="F23" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="I23" s="31" t="s">
         <v>117</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H23" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="I23" s="31" t="s">
-        <v>118</v>
       </c>
       <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B24" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>8</v>
@@ -3123,28 +3137,28 @@
         <v>20</v>
       </c>
       <c r="F24" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="I24" s="31" t="s">
         <v>121</v>
-      </c>
-      <c r="G24" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="I24" s="31" t="s">
-        <v>122</v>
       </c>
       <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B25" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D25" s="28" t="s">
         <v>8</v>
@@ -3153,118 +3167,118 @@
         <v>20</v>
       </c>
       <c r="F25" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="I25" s="31" t="s">
         <v>125</v>
-      </c>
-      <c r="G25" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="H25" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="I25" s="31" t="s">
-        <v>126</v>
       </c>
       <c r="J25" s="31"/>
     </row>
     <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B26" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I26" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J26" s="31"/>
     </row>
     <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B27" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F27" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="G27" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H27" s="35" t="s">
-        <v>133</v>
-      </c>
       <c r="I27" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B28" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H28" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I28" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D29" s="28" t="s">
         <v>8</v>
@@ -3273,28 +3287,28 @@
         <v>20</v>
       </c>
       <c r="F29" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="H29" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="G29" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="H29" s="34" t="s">
+      <c r="I29" s="31" t="s">
         <v>145</v>
-      </c>
-      <c r="I29" s="31" t="s">
-        <v>146</v>
       </c>
       <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D30" s="28" t="s">
         <v>8</v>
@@ -3303,28 +3317,28 @@
         <v>20</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H30" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I30" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D31" s="28" t="s">
         <v>8</v>
@@ -3333,28 +3347,28 @@
         <v>20</v>
       </c>
       <c r="F31" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H31" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="I31" s="31" t="s">
         <v>152</v>
-      </c>
-      <c r="G31" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H31" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="I31" s="31" t="s">
-        <v>153</v>
       </c>
       <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B32" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D32" s="28" t="s">
         <v>8</v>
@@ -3363,28 +3377,28 @@
         <v>20</v>
       </c>
       <c r="F32" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H32" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="I32" s="31" t="s">
         <v>152</v>
-      </c>
-      <c r="G32" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H32" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="I32" s="31" t="s">
-        <v>153</v>
       </c>
       <c r="J32" s="31"/>
     </row>
     <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B33" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D33" s="28" t="s">
         <v>8</v>
@@ -3393,136 +3407,136 @@
         <v>20</v>
       </c>
       <c r="F33" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G33" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H33" s="41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I33" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J33" s="31"/>
     </row>
     <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B34" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F34" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H34" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="I34" s="31" t="s">
         <v>164</v>
-      </c>
-      <c r="G34" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H34" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="I34" s="31" t="s">
-        <v>165</v>
       </c>
       <c r="J34" s="31"/>
     </row>
     <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B35" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F35" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="G35" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H35" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="I35" s="31" t="s">
         <v>164</v>
-      </c>
-      <c r="G35" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H35" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="I35" s="31" t="s">
-        <v>165</v>
       </c>
       <c r="J35" s="31"/>
     </row>
     <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F36" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G36" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H36" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I36" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J36" s="31"/>
     </row>
     <row r="37" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B37" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E37" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F37" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="I37" s="34" t="s">
         <v>171</v>
-      </c>
-      <c r="G37" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="H37" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="I37" s="34" t="s">
-        <v>172</v>
       </c>
       <c r="J37" s="31"/>
     </row>

</xml_diff>

<commit_message>
630922 Updated for T33
</commit_message>
<xml_diff>
--- a/Test/Build 6/TAS eBill Defect Log IB_2.0_608.xlsx
+++ b/Test/Build 6/TAS eBill Defect Log IB_2.0_608.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaispbalchj\Documents\eBilling Docs\Build 5&amp;6\Docs\Defect Log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaispbalchj\Documents\eBilling Docs\Build 5&amp;6\Docs\All\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="177">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -580,7 +580,7 @@
   </si>
   <si>
     <r>
-      <t>Version 2.0</t>
+      <t>Version 3.0</t>
     </r>
     <r>
       <rPr>
@@ -594,7 +594,10 @@
     </r>
   </si>
   <si>
-    <t>Updated for Blds 5/6 retesting effort</t>
+    <t>Updated for testing of T32</t>
+  </si>
+  <si>
+    <t>Updated for testing of T33</t>
   </si>
 </sst>
 </file>
@@ -2128,7 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:H26"/>
     </sheetView>
   </sheetViews>
@@ -2276,7 +2279,7 @@
   <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2345,10 +2348,18 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
+      <c r="A7" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="13">
+        <v>3</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>

</xml_diff>

<commit_message>
753304 Updated for IOC exit
</commit_message>
<xml_diff>
--- a/Test/Build 6/TAS eBill Defect Log IB_2.0_608.xlsx
+++ b/Test/Build 6/TAS eBill Defect Log IB_2.0_608.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaispbalchj\Documents\eBilling Docs\Build 5&amp;6\Docs\All\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\eBilling Docs\Build 5&amp;6\Docs\All\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62F5583-6331-49B4-B907-8531351081E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10344" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10344" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="196">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -576,11 +577,62 @@
     <t>UAT - CMN Ox question 4  - piece 4 now holds piece 4 and  5</t>
   </si>
   <si>
-    <t>October 2018</t>
+    <t>DE801</t>
+  </si>
+  <si>
+    <t>CIT - CIT - Rate type not deleteing correctly US2599</t>
+  </si>
+  <si>
+    <t>TC3384: CIT - CMN Oxygen and EPN Nutrition – Editing Procedure Types US3</t>
+  </si>
+  <si>
+    <t>6/11/2018 Found in IB*2.0*608_T31</t>
+  </si>
+  <si>
+    <t>7/9/2018 Verified in IB*2.0*608_T32</t>
+  </si>
+  <si>
+    <t>DE929</t>
+  </si>
+  <si>
+    <t>CIT - US3 FRM segment field FRM-7 is sending empty spaces</t>
+  </si>
+  <si>
+    <t>8/29/2018 Found in IB*2.0*608_T31</t>
+  </si>
+  <si>
+    <t>9/4/2018 Verified in IB*2.0*608_T32</t>
+  </si>
+  <si>
+    <t>IOC - One-Time report generated and sent twice in Production Env US1909</t>
+  </si>
+  <si>
+    <t>DE1055</t>
+  </si>
+  <si>
+    <t>11/29/2018 Found in IB*2.0*608_T33</t>
+  </si>
+  <si>
+    <t>1/8/2019 Verified in IB*2.0*608_T34</t>
+  </si>
+  <si>
+    <t>DE1070</t>
+  </si>
+  <si>
+    <t>IOC - SNF Piece 5 is transmitting incorrectly</t>
+  </si>
+  <si>
+    <t>US9 - Transmitting SNF Claims with Appropriate Revenue (USEB-16)</t>
+  </si>
+  <si>
+    <t>1/7/2019 Found in IB*2.0*608_T33</t>
+  </si>
+  <si>
+    <t>March 2019</t>
   </si>
   <si>
     <r>
-      <t>Version 3.0</t>
+      <t>Version 4.0</t>
     </r>
     <r>
       <rPr>
@@ -594,16 +646,22 @@
     </r>
   </si>
   <si>
+    <t>October 2018</t>
+  </si>
+  <si>
     <t>Updated for testing of T32</t>
   </si>
   <si>
     <t>Updated for testing of T33</t>
+  </si>
+  <si>
+    <t>Updated with results through final build testing of T36</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1310,7 +1368,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
@@ -1429,6 +1487,12 @@
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="35" borderId="11" xfId="42" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1488,7 +1552,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1797,12 +1861,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Revision_History" displayName="Revision_History" ref="A3:D14" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Revision_History" displayName="Revision_History" ref="A3:D16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="3"/>
-    <tableColumn id="2" name="Version" dataDxfId="2"/>
-    <tableColumn id="3" name="Description" dataDxfId="1"/>
-    <tableColumn id="4" name="Author" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Version" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Author" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2128,7 +2192,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:H34"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
@@ -2143,31 +2207,31 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
@@ -2212,16 +2276,16 @@
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="46" t="s">
-        <v>173</v>
-      </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
+      <c r="A23" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
@@ -2232,16 +2296,16 @@
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="47" t="s">
-        <v>174</v>
-      </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
+      <c r="A26" s="49" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
     </row>
     <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
@@ -2275,29 +2339,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D8" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="7" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" style="17" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
     </row>
     <row r="3" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -2327,45 +2391,53 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="11"/>
+    <row r="5" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="44">
+        <v>2</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="13">
-        <v>2</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="A6" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="44">
+        <v>3</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" s="13">
-        <v>3</v>
+        <v>190</v>
+      </c>
+      <c r="B7" s="10">
+        <v>4</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
@@ -2398,10 +2470,22 @@
       <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2416,11 +2500,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3551,40 +3635,184 @@
       </c>
       <c r="J37" s="31"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
+    <row r="38" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H38" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="I38" s="34" t="s">
+        <v>177</v>
+      </c>
       <c r="J38" s="31"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
+    <row r="39" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="I39" s="34" t="s">
+        <v>181</v>
+      </c>
       <c r="J39" s="31"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="38"/>
+    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="G40" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I40" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="J40" s="31"/>
+    </row>
+    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="G41" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="H41" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="I41" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="J41" s="31"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="31"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="31"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="31"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="31"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="31"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="31"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B46" s="38"/>
     </row>
   </sheetData>
   <sortState ref="A2:H12">
     <sortCondition descending="1" ref="A2:A12"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" location="/79590444732d/detail/defect/149014856112" display="https://rally1.rallydev.com/ - /79590444732d/detail/defect/149014856112"/>
-    <hyperlink ref="A2" r:id="rId2" location="/79590444732d/detail/defect/148456306180" display="/79590444732d/detail/defect/148456306180"/>
+    <hyperlink ref="A3" r:id="rId1" location="/79590444732d/detail/defect/149014856112" display="https://rally1.rallydev.com/ - /79590444732d/detail/defect/149014856112" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="/79590444732d/detail/defect/148456306180" display="/79590444732d/detail/defect/148456306180" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>